<commit_message>
second commit in functional_testing
</commit_message>
<xml_diff>
--- a/Functional_Testing_Travel_Website.xlsx
+++ b/Functional_Testing_Travel_Website.xlsx
@@ -8,20 +8,21 @@
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" state="hidden" r:id="rId1"/>
-    <sheet name="TEST SCENARIO" sheetId="1" r:id="rId2"/>
-    <sheet name="TEST CASES" sheetId="2" r:id="rId3"/>
-    <sheet name="DEFECT REPORT" sheetId="3" r:id="rId4"/>
-    <sheet name="RTM" sheetId="4" r:id="rId5"/>
+    <sheet name="Project Summary" sheetId="6" r:id="rId2"/>
+    <sheet name="TEST SCENARIO" sheetId="1" r:id="rId3"/>
+    <sheet name="TEST CASES" sheetId="2" r:id="rId4"/>
+    <sheet name="DEFECT REPORT" sheetId="3" r:id="rId5"/>
+    <sheet name="RTM" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TEST CASES'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'TEST CASES'!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="154">
   <si>
     <t>Module</t>
   </si>
@@ -35,9 +36,6 @@
     <t>Test case description</t>
   </si>
   <si>
-    <t>Prerequisites</t>
-  </si>
-  <si>
     <t>Steps to execute</t>
   </si>
   <si>
@@ -47,9 +45,6 @@
     <t>Actual results</t>
   </si>
   <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
     <t>Defect id</t>
   </si>
   <si>
@@ -59,9 +54,6 @@
     <t>Serial no.</t>
   </si>
   <si>
-    <t>Reproducible (yes/no)</t>
-  </si>
-  <si>
     <t>Steps to reproduce</t>
   </si>
   <si>
@@ -410,9 +402,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Deva K</t>
-  </si>
-  <si>
     <t>Assigned</t>
   </si>
   <si>
@@ -441,6 +430,60 @@
   </si>
   <si>
     <t>TC009</t>
+  </si>
+  <si>
+    <t>Executed QA Name</t>
+  </si>
+  <si>
+    <t>DevaKiskar</t>
+  </si>
+  <si>
+    <t>Pre-Conditions</t>
+  </si>
+  <si>
+    <t>Project  Name</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Reveiwed By</t>
+  </si>
+  <si>
+    <t>Reveiwed Date</t>
+  </si>
+  <si>
+    <t>KSRTC Travels(web app)</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>12.04.2023</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Reproducable (yes/no)</t>
+  </si>
+  <si>
+    <t>From date test box</t>
+  </si>
+  <si>
+    <t>To date test box</t>
   </si>
 </sst>
 </file>
@@ -544,6 +587,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Fields"/>
+    <tableColumn id="2" name="Details"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -927,7 +981,7 @@
     <row r="6" spans="1:15">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -947,7 +1001,7 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -966,7 +1020,7 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -985,7 +1039,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1004,7 +1058,7 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1023,7 +1077,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1042,7 +1096,7 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1201,16 +1255,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="59.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
@@ -1221,13 +1345,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1235,478 +1359,155 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
         <v>61</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>69</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" customWidth="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="30">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30">
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H5" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="E6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="E7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="E9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="E10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="E11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30">
-      <c r="A12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30">
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" t="s">
-        <v>114</v>
-      </c>
-      <c r="H13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="E14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="E15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30">
-      <c r="A16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="30">
-      <c r="B17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" t="s">
-        <v>124</v>
-      </c>
-      <c r="H17" t="s">
-        <v>84</v>
-      </c>
-      <c r="I17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="E18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="E19" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1717,10 +1518,416 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="B13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" t="s">
+        <v>150</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="E15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="30">
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" t="s">
+        <v>149</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="E19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1740,37 +1947,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30">
@@ -1778,41 +1985,41 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I2" s="7">
         <v>44832</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="E3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="E4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30">
@@ -1820,46 +2027,46 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I5" s="7">
         <v>44832</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="E6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="E7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="E8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1867,46 +2074,46 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I9" s="7">
         <v>44832</v>
       </c>
       <c r="J9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="E10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="E11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="E12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1915,7 +2122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1934,22 +2141,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1957,19 +2164,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1977,19 +2184,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1997,19 +2204,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2017,19 +2224,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2037,19 +2244,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2057,19 +2264,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2077,19 +2284,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2097,19 +2304,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2117,19 +2324,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>